<commit_message>
Use nicer fonts in Info.*
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -62,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -83,6 +83,24 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cascadia Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Cascadia Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,13 +145,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -153,75 +183,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="76.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="77.32"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>50000</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>958</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="2" t="n">
         <v>50000</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <v>958</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2" t="n">
         <v>219</v>
       </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Add language code information to the help
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -185,14 +185,14 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="76.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="77.32"/>
   </cols>
@@ -230,7 +230,7 @@
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>958</v>
+        <v>1035</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -245,7 +245,7 @@
         <v>50000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>958</v>
+        <v>1034</v>
       </c>
       <c r="E4" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add 'code' after 'target language'
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -186,10 +186,10 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.22"/>
@@ -230,7 +230,7 @@
         <v>50000</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1035</v>
+        <v>1040</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -245,7 +245,7 @@
         <v>50000</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="E4" s="1"/>
     </row>

</xml_diff>